<commit_message>
Using real objects for export/publish tests.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -15,43 +15,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
-  <si>
-    <t>1.1.0</t>
-  </si>
-  <si>
-    <t>2.1.0</t>
-  </si>
-  <si>
-    <t>2.1.1</t>
-  </si>
-  <si>
-    <t>CHECK_PUBLISHED_CONTENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heading
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello, world!
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Heading 2
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-Hello, world!
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc 123
-</t>
+    <t>REF123</t>
+  </si>
+  <si>
+    <t>REQ001</t>
+  </si>
+  <si>
+    <t>REQ002</t>
+  </si>
+  <si>
+    <t>REQ003</t>
+  </si>
+  <si>
+    <t>REQ004</t>
+  </si>
+  <si>
+    <t>REQ2-001</t>
+  </si>
+  <si>
+    <t>SYS001, SYS002</t>
   </si>
   <si>
     <t>active</t>
@@ -73,24 +64,6 @@
   </si>
   <si>
     <t>ref</t>
-  </si>
-  <si>
-    <t>req1</t>
-  </si>
-  <si>
-    <t>req2</t>
-  </si>
-  <si>
-    <t>req3</t>
-  </si>
-  <si>
-    <t>req4</t>
-  </si>
-  <si>
-    <t>sys1</t>
-  </si>
-  <si>
-    <t>sys3</t>
   </si>
   <si>
     <t>text</t>
@@ -427,169 +400,267 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="B1">
-        <v>11</v>
-      </c>
-      <c t="s" r="C1">
-        <v>21</v>
-      </c>
-      <c t="s" r="D1">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="E1">
-        <v>12</v>
-      </c>
-      <c t="s" r="F1">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="G1">
-        <v>9</v>
-      </c>
-      <c t="s" r="H1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c t="s" r="A2">
-        <v>17</v>
-      </c>
-      <c t="s" r="B2">
-        <v>0</v>
-      </c>
-      <c t="s" r="C2">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="E2">
-        <v>20</v>
-      </c>
-      <c t="b" r="F2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G2">
-        <v>0</v>
-      </c>
-      <c t="b" r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c t="s" r="A3">
-        <v>17</v>
-      </c>
-      <c t="n" r="B3">
-        <v>1.2</v>
-      </c>
-      <c t="s" r="C3">
+      <c r="B5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="E3">
-        <v>20</v>
-      </c>
-      <c t="b" r="F3">
-        <v>1</v>
-      </c>
-      <c t="b" r="G3">
-        <v>0</v>
-      </c>
-      <c t="b" r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c t="s" r="A4">
-        <v>15</v>
-      </c>
-      <c t="n" r="B4">
-        <v>1.1</v>
-      </c>
-      <c t="s" r="C4">
-        <v>7</v>
-      </c>
-      <c t="b" r="F4">
-        <v>1</v>
-      </c>
-      <c t="b" r="G4">
-        <v>0</v>
-      </c>
-      <c t="b" r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c t="s" r="A5">
-        <v>16</v>
-      </c>
-      <c t="n" r="B5">
-        <v>2</v>
-      </c>
-      <c t="b" r="F5">
-        <v>1</v>
-      </c>
-      <c t="b" r="G5">
-        <v>0</v>
-      </c>
-      <c t="b" r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c t="s" r="A6">
-        <v>18</v>
-      </c>
-      <c t="s" r="B6">
-        <v>2</v>
-      </c>
-      <c t="s" r="D6">
-        <v>3</v>
-      </c>
-      <c t="b" r="F6">
-        <v>1</v>
-      </c>
-      <c t="b" r="G6">
-        <v>0</v>
-      </c>
-      <c t="b" r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c t="s" r="A7">
-        <v>16</v>
-      </c>
-      <c t="s" r="B7">
-        <v>1</v>
-      </c>
-      <c t="s" r="C7">
-        <v>5</v>
-      </c>
-      <c t="s" r="E7">
-        <v>19</v>
-      </c>
-      <c t="b" r="F7">
-        <v>1</v>
-      </c>
-      <c t="b" r="G7">
-        <v>0</v>
-      </c>
-      <c t="b" r="H7">
-        <v>0</v>
+      <c r="B11" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" header="0.5" right="0.75" footer="0.5" top="1" left="0.75"/>
+  <pageMargins top="1" left="0.75" right="0.75" footer="0.5" header="0.5" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made the headings bold.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="124519"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>1.2.3</t>
   </si>
@@ -72,10 +71,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,16 +107,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,6 +201,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -223,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,157 +412,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row spans="1:8" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C2">
-        <v>1</v>
-      </c>
-      <c t="s" r="E2">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c t="b" r="F2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G2">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H2">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
-      <c t="s" r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3">
         <v>1.4</v>
       </c>
-      <c t="s" r="C3">
-        <v>1</v>
-      </c>
-      <c t="s" r="D3">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c t="b" r="F3">
-        <v>1</v>
-      </c>
-      <c t="b" r="G3">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H3">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4">
         <v>1.6</v>
       </c>
-      <c t="s" r="C4">
-        <v>1</v>
-      </c>
-      <c t="b" r="F4">
-        <v>1</v>
-      </c>
-      <c t="b" r="G4">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H4">
+      <c r="H4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c t="n" r="B5">
+      <c r="B5">
         <v>2.1</v>
       </c>
-      <c t="s" r="C5">
-        <v>1</v>
-      </c>
-      <c t="b" r="F5">
-        <v>1</v>
-      </c>
-      <c t="b" r="G5">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H5">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6">
         <v>2.1</v>
       </c>
-      <c t="s" r="C6">
-        <v>1</v>
-      </c>
-      <c t="s" r="E6">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c t="b" r="F6">
-        <v>1</v>
-      </c>
-      <c t="b" r="G6">
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H6">
+      <c r="H6" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" header="0.5" top="1" right="0.75" left="0.75" footer="0.5"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests and fixed Item.data loading bug.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames>
+    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$H$1</s:definedName>
+  </s:definedNames>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>1.2.3</t>
   </si>
@@ -41,7 +47,8 @@
     <t>REQ2-001</t>
   </si>
   <si>
-    <t>SYS001, SYS002</t>
+    <t>SYS001,
+SYS002</t>
   </si>
   <si>
     <t>active</t>
@@ -71,8 +78,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,12 +89,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11.0"/>
+      <color rgb="00000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,22 +114,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -201,7 +208,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -236,7 +242,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,155 +417,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <pane state="frozen" topLeftCell="A2" activePane="bottomLeft" ySplit="1"/>
+      <selection sqref="A1" pane="bottomLeft" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.5" min="1" max="1"/>
+    <col width="8.5" min="2" max="2"/>
+    <col width="16.5" min="3" max="3"/>
+    <col width="9.5" min="4" max="4"/>
+    <col width="10.5" min="5" max="5"/>
+    <col width="9.5" min="6" max="6"/>
+    <col width="10.5" min="7" max="7"/>
+    <col width="12.5" min="8" max="8"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s"/>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s"/>
+      <c r="E4" s="2" t="s"/>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s"/>
+      <c r="E5" s="2" t="s"/>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
+      <c r="B6" s="2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s"/>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1.4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1.6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2.1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>2.1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
+      <c r="H6" s="2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <autoFilter ref="A1:H1"/>
+  <pageMargins left="0.75" right="0.75" top="1" header="0.5" footer="0.5" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved type conversion to file functions.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -17,12 +17,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t/>
   </si>
   <si>
     <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>2.1</t>
   </si>
   <si>
     <t xml:space="preserve">Hello, world!
@@ -417,18 +426,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane state="frozen" topLeftCell="A2" activePane="bottomLeft" ySplit="1"/>
-      <selection sqref="A1" pane="bottomLeft" activeCell="A1"/>
+      <pane activePane="bottomLeft" ySplit="1" topLeftCell="A2" state="frozen"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
     <col width="11.5" min="1" max="1"/>
     <col width="8.5" min="2" max="2"/>
@@ -440,152 +449,152 @@
     <col width="12.5" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row spans="1:8" r="1">
+      <c t="s" s="1" r="A1">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:8" r="2">
+      <c t="s" s="2" r="A2">
+        <v>7</v>
+      </c>
+      <c t="s" s="2" r="B2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="C2">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D2"/>
+      <c t="s" s="2" r="E2">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c t="b" s="2" r="F2">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G2">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:8" r="3">
+      <c t="s" s="2" r="A3">
+        <v>9</v>
+      </c>
+      <c t="s" s="2" r="B3">
+        <v>2</v>
+      </c>
+      <c t="s" s="2" r="C3">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D3">
+        <v>6</v>
+      </c>
+      <c t="s" s="2" r="E3">
+        <v>7</v>
+      </c>
+      <c t="b" s="2" r="F3">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G3">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:8" r="4">
+      <c t="s" s="2" r="A4">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c t="s" s="2" r="B4">
+        <v>3</v>
+      </c>
+      <c t="s" s="2" r="C4">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D4"/>
+      <c t="s" s="2" r="E4"/>
+      <c t="b" s="2" r="F4">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G4">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:8" r="5">
+      <c t="s" s="2" r="A5">
+        <v>8</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>4</v>
+      </c>
+      <c t="s" s="2" r="C5">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D5"/>
+      <c t="s" s="2" r="E5"/>
+      <c t="b" s="2" r="F5">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G5">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row spans="1:8" r="6">
+      <c t="s" s="2" r="A6">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c t="s" s="2" r="B6">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
+      <c t="s" s="2" r="C6">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D6"/>
+      <c t="s" s="2" r="E6">
+        <v>7</v>
+      </c>
+      <c t="b" s="2" r="F6">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G6">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="b">
+      <c t="b" s="2" r="H6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
-  <pageMargins left="0.75" right="0.75" top="1" header="0.5" footer="0.5" bottom="1"/>
+  <pageMargins footer="0.5" right="0.75" left="0.75" top="1" bottom="1" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Forced UTF-8 in output files.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -430,175 +430,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" state="frozen" activePane="bottomLeft" topLeftCell="A2"/>
-      <selection sqref="A1" pane="bottomLeft" activeCell="A1"/>
+      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col max="1" min="1" width="11.5"/>
-    <col max="2" min="2" width="8.5"/>
-    <col max="3" min="3" width="20.5"/>
-    <col max="4" min="4" width="9.5"/>
-    <col max="5" min="5" width="10.5"/>
-    <col max="6" min="6" width="9.5"/>
-    <col max="7" min="7" width="10.5"/>
-    <col max="8" min="8" width="12.5"/>
+    <col width="11.5" min="1" max="1"/>
+    <col width="8.5" min="2" max="2"/>
+    <col width="20.5" min="3" max="3"/>
+    <col width="9.5" min="4" max="4"/>
+    <col width="10.5" min="5" max="5"/>
+    <col width="9.5" min="6" max="6"/>
+    <col width="10.5" min="7" max="7"/>
+    <col width="12.5" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row spans="1:8" r="1">
+      <c t="s" r="A1" s="1">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c t="s" r="B1" s="1">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c t="s" r="C1" s="1">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c t="s" r="D1" s="1">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c t="s" r="E1" s="1">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c t="s" r="F1" s="1">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c t="s" r="G1" s="1">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c t="s" r="H1" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+    <row spans="1:8" r="2">
+      <c t="s" r="A2" s="2">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c t="s" r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
+      <c t="s" r="D2" s="2"/>
+      <c t="s" r="E2" s="2">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
+      <c t="b" r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="b">
+      <c t="b" r="H2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+    <row spans="1:8" r="3">
+      <c t="s" r="A3" s="2">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c t="s" r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c t="s" r="C3" s="2">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c t="s" r="D3" s="2">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c t="s" r="E3" s="2">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="b">
+      <c t="b" r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="b">
+      <c t="b" r="H3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+    <row spans="1:8" r="4">
+      <c t="s" r="A4" s="2">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c t="s" r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c t="s" r="C4" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="b">
+      <c t="s" r="D4" s="2"/>
+      <c t="s" r="E4" s="2"/>
+      <c t="b" r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="b">
+      <c t="b" r="H4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
+    <row spans="1:8" r="5">
+      <c t="s" r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c t="s" r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c t="s" r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
+      <c t="s" r="D5" s="2"/>
+      <c t="s" r="E5" s="2"/>
+      <c t="b" r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="b">
+      <c t="b" r="H5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
+    <row spans="1:8" r="6">
+      <c t="s" r="A6" s="2">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c t="s" r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c t="s" r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
+      <c t="s" r="D6" s="2"/>
+      <c t="s" r="E6" s="2">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
+      <c t="b" r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="b">
+      <c t="b" r="H6" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
-  <pageMargins header="0.5" left="0.75" right="0.75" footer="0.5" top="1" bottom="1"/>
+  <pageMargins bottom="1" top="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed failing export tests. Import still failing.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -10,14 +10,14 @@
     <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$H$1</s:definedName>
+    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$I$1</s:definedName>
   </s:definedNames>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t/>
   </si>
@@ -56,7 +56,7 @@
     <t>REQ2-001</t>
   </si>
   <si>
-    <t>SYS001,
+    <t>SYS001
 SYS002</t>
   </si>
   <si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>ref</t>
+  </si>
+  <si>
+    <t>reviewed</t>
   </si>
   <si>
     <t>text</t>
@@ -430,30 +433,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane topLeftCell="A2" state="frozen" ySplit="1" activePane="bottomLeft"/>
+      <selection activeCell="A1" sqref="A1" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
     <col width="11.5" min="1" max="1"/>
     <col width="8.5" min="2" max="2"/>
     <col width="20.5" min="3" max="3"/>
     <col width="9.5" min="4" max="4"/>
-    <col width="10.5" min="5" max="5"/>
+    <col width="9.5" min="5" max="5"/>
     <col width="9.5" min="6" max="6"/>
     <col width="10.5" min="7" max="7"/>
     <col width="12.5" min="8" max="8"/>
+    <col width="11.5" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row spans="1:8" r="1">
+    <row r="1" spans="1:9">
       <c t="s" r="A1" s="1">
         <v>16</v>
       </c>
@@ -461,7 +465,7 @@
         <v>17</v>
       </c>
       <c t="s" r="C1" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c t="s" r="D1" s="1">
         <v>20</v>
@@ -478,8 +482,11 @@
       <c t="s" r="H1" s="1">
         <v>19</v>
       </c>
+      <c t="s" r="I1" s="1">
+        <v>21</v>
+      </c>
     </row>
-    <row spans="1:8" r="2">
+    <row r="2" spans="1:9">
       <c t="s" r="A2" s="2">
         <v>7</v>
       </c>
@@ -502,8 +509,11 @@
       <c t="b" r="H2" s="2">
         <v>1</v>
       </c>
+      <c t="b" r="I2" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row spans="1:8" r="3">
+    <row r="3" spans="1:9">
       <c t="s" r="A3" s="2">
         <v>9</v>
       </c>
@@ -528,8 +538,11 @@
       <c t="b" r="H3" s="2">
         <v>1</v>
       </c>
+      <c t="b" r="I3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row spans="1:8" r="4">
+    <row r="4" spans="1:9">
       <c t="s" r="A4" s="2">
         <v>10</v>
       </c>
@@ -550,8 +563,11 @@
       <c t="b" r="H4" s="2">
         <v>1</v>
       </c>
+      <c t="b" r="I4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row spans="1:8" r="5">
+    <row r="5" spans="1:9">
       <c t="s" r="A5" s="2">
         <v>8</v>
       </c>
@@ -572,8 +588,11 @@
       <c t="b" r="H5" s="2">
         <v>1</v>
       </c>
+      <c t="b" r="I5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row spans="1:8" r="6">
+    <row r="6" spans="1:9">
       <c t="s" r="A6" s="2">
         <v>11</v>
       </c>
@@ -596,9 +615,12 @@
       <c t="b" r="H6" s="2">
         <v>1</v>
       </c>
+      <c t="b" r="I6" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
-  <pageMargins bottom="1" top="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
+  <autoFilter ref="A1:I1"/>
+  <pageMargins top="1" left="0.75" bottom="1" header="0.5" right="0.75" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed test failures (still lacking coverage).
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -57,7 +57,7 @@
   </si>
   <si>
     <t>SYS001
-SYS002</t>
+SYS002:abc123</t>
   </si>
   <si>
     <t xml:space="preserve">Unicode: -40° ±1%
@@ -433,194 +433,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane topLeftCell="A2" state="frozen" ySplit="1" activePane="bottomLeft"/>
-      <selection activeCell="A1" sqref="A1" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" min="1" max="1"/>
-    <col width="8.5" min="2" max="2"/>
-    <col width="20.5" min="3" max="3"/>
-    <col width="9.5" min="4" max="4"/>
-    <col width="9.5" min="5" max="5"/>
-    <col width="9.5" min="6" max="6"/>
-    <col width="10.5" min="7" max="7"/>
-    <col width="12.5" min="8" max="8"/>
-    <col width="11.5" min="9" max="9"/>
+    <col min="1" width="11.5" max="1"/>
+    <col min="2" width="8.5" max="2"/>
+    <col min="3" width="20.5" max="3"/>
+    <col min="4" width="9.5" max="4"/>
+    <col min="5" width="16.5" max="5"/>
+    <col min="6" width="9.5" max="6"/>
+    <col min="7" width="10.5" max="7"/>
+    <col min="8" width="12.5" max="8"/>
+    <col min="9" width="11.5" max="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c t="s" r="A1" s="1">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="D1" s="1">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="E1" s="1">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="F1" s="1">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="G1" s="1">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="H1" s="1">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="I1" s="1">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c t="s" r="A2" s="2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="C2" s="2">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="D2" s="2"/>
-      <c t="s" r="E2" s="2">
+      <c r="D2" s="2" t="s"/>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="b" r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G2" s="2">
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="I2" s="2">
-        <v>0</v>
-      </c>
+      <c r="H2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s"/>
     </row>
     <row r="3" spans="1:9">
-      <c t="s" r="A3" s="2">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="B3" s="2">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="C3" s="2">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="D3" s="2">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="E3" s="2">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="b" r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G3" s="2">
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="I3" s="2">
-        <v>0</v>
-      </c>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s"/>
     </row>
     <row r="4" spans="1:9">
-      <c t="s" r="A4" s="2">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="B4" s="2">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="C4" s="2">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="D4" s="2"/>
-      <c t="s" r="E4" s="2"/>
-      <c t="b" r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G4" s="2">
+      <c r="D4" s="2" t="s"/>
+      <c r="E4" s="2" t="s"/>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="I4" s="2">
-        <v>0</v>
-      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s"/>
     </row>
     <row r="5" spans="1:9">
-      <c t="s" r="A5" s="2">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="B5" s="2">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="C5" s="2">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="D5" s="2"/>
-      <c t="s" r="E5" s="2"/>
-      <c t="b" r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G5" s="2">
+      <c r="D5" s="2" t="s"/>
+      <c r="E5" s="2" t="s"/>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="I5" s="2">
-        <v>0</v>
-      </c>
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s"/>
     </row>
     <row r="6" spans="1:9">
-      <c t="s" r="A6" s="2">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="B6" s="2">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="C6" s="2">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="D6" s="2"/>
-      <c t="s" r="E6" s="2">
+      <c r="D6" s="2" t="s"/>
+      <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="b" r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G6" s="2">
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="I6" s="2">
-        <v>0</v>
-      </c>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins top="1" left="0.75" bottom="1" header="0.5" right="0.75" footer="0.5"/>
+  <pageMargins footer="0.5" right="0.75" top="1" left="0.75" header="0.5" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored stamps into a Stamp class.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t/>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>b5fbcc355112791bbcd2ea881c7c5f81</t>
   </si>
   <si>
     <t>derived</t>
@@ -435,182 +438,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane ySplit="1" activePane="bottomLeft" state="frozen" topLeftCell="A2"/>
+      <selection activeCell="A1" sqref="A1" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
-    <col min="1" width="11.5" max="1"/>
-    <col min="2" width="8.5" max="2"/>
-    <col min="3" width="20.5" max="3"/>
-    <col min="4" width="9.5" max="4"/>
-    <col min="5" width="16.5" max="5"/>
-    <col min="6" width="9.5" max="6"/>
-    <col min="7" width="10.5" max="7"/>
-    <col min="8" width="12.5" max="8"/>
-    <col min="9" width="11.5" max="9"/>
+    <col width="11.5" max="1" min="1"/>
+    <col width="8.5" max="2" min="2"/>
+    <col width="20.5" max="3" min="3"/>
+    <col width="9.5" max="4" min="4"/>
+    <col width="16.5" max="5" min="5"/>
+    <col width="9.5" max="6" min="6"/>
+    <col width="10.5" max="7" min="7"/>
+    <col width="12.5" max="8" min="8"/>
+    <col width="35.5" max="9" min="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row spans="1:9" r="1">
+      <c t="s" s="1" r="A1">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="G1">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c t="s" s="1" r="H1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="I1">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row spans="1:9" r="2">
+      <c t="s" s="2" r="A2">
+        <v>7</v>
+      </c>
+      <c t="s" s="2" r="B2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="C2">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D2"/>
+      <c t="s" s="2" r="E2">
+        <v>12</v>
+      </c>
+      <c t="b" s="2" r="F2">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G2">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I2"/>
+    </row>
+    <row spans="1:9" r="3">
+      <c t="s" s="2" r="A3">
+        <v>9</v>
+      </c>
+      <c t="s" s="2" r="B3">
+        <v>2</v>
+      </c>
+      <c t="s" s="2" r="C3">
+        <v>13</v>
+      </c>
+      <c t="s" s="2" r="D3">
+        <v>6</v>
+      </c>
+      <c t="s" s="2" r="E3">
+        <v>7</v>
+      </c>
+      <c t="b" s="2" r="F3">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G3">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H3">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I3"/>
+    </row>
+    <row spans="1:9" r="4">
+      <c t="s" s="2" r="A4">
+        <v>10</v>
+      </c>
+      <c t="s" s="2" r="B4">
+        <v>3</v>
+      </c>
+      <c t="s" s="2" r="C4">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D4"/>
+      <c t="s" s="2" r="E4"/>
+      <c t="b" s="2" r="F4">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G4">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H4">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I4"/>
+    </row>
+    <row spans="1:9" r="5">
+      <c t="s" s="2" r="A5">
+        <v>8</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>4</v>
+      </c>
+      <c t="s" s="2" r="C5">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D5"/>
+      <c t="s" s="2" r="E5"/>
+      <c t="b" s="2" r="F5">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G5">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H5">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I5">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+    <row spans="1:9" r="6">
+      <c t="s" s="2" r="A6">
+        <v>11</v>
+      </c>
+      <c t="s" s="2" r="B6">
+        <v>4</v>
+      </c>
+      <c t="s" s="2" r="C6">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D6"/>
+      <c t="s" s="2" r="E6">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
+      <c t="b" s="2" r="F6">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G6">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s"/>
+      <c t="b" s="2" r="H6">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins footer="0.5" right="0.75" top="1" left="0.75" header="0.5" bottom="1"/>
+  <pageMargins bottom="1" right="0.75" footer="0.5" top="1" header="0.5" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merged branch 'master' into branch 'server'.
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -10,14 +10,14 @@
     <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$H$1</s:definedName>
+    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$I$1</s:definedName>
   </s:definedNames>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t/>
   </si>
@@ -56,8 +56,8 @@
     <t>REQ2-001</t>
   </si>
   <si>
-    <t>SYS001,
-SYS002</t>
+    <t>SYS001
+SYS002:abc123</t>
   </si>
   <si>
     <t xml:space="preserve">Unicode: -40° ±1%
@@ -67,6 +67,9 @@
     <t>active</t>
   </si>
   <si>
+    <t>b5fbcc355112791bbcd2ea881c7c5f81</t>
+  </si>
+  <si>
     <t>derived</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>ref</t>
+  </si>
+  <si>
+    <t>reviewed</t>
   </si>
   <si>
     <t>text</t>
@@ -432,173 +438,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane ySplit="1" activePane="bottomLeft" state="frozen" topLeftCell="A2"/>
+      <selection activeCell="A1" sqref="A1" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
-    <col width="11.5" min="1" max="1"/>
-    <col width="8.5" min="2" max="2"/>
-    <col width="20.5" min="3" max="3"/>
-    <col width="9.5" min="4" max="4"/>
-    <col width="10.5" min="5" max="5"/>
-    <col width="9.5" min="6" max="6"/>
-    <col width="10.5" min="7" max="7"/>
-    <col width="12.5" min="8" max="8"/>
+    <col width="11.5" max="1" min="1"/>
+    <col width="8.5" max="2" min="2"/>
+    <col width="20.5" max="3" min="3"/>
+    <col width="9.5" max="4" min="4"/>
+    <col width="16.5" max="5" min="5"/>
+    <col width="9.5" max="6" min="6"/>
+    <col width="10.5" max="7" min="7"/>
+    <col width="12.5" max="8" min="8"/>
+    <col width="35.5" max="9" min="9"/>
   </cols>
   <sheetData>
-    <row spans="1:8" r="1">
-      <c t="s" r="A1" s="1">
+    <row spans="1:9" r="1">
+      <c t="s" s="1" r="A1">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="G1">
         <v>16</v>
       </c>
-      <c t="s" r="B1" s="1">
-        <v>17</v>
-      </c>
-      <c t="s" r="C1" s="1">
-        <v>21</v>
-      </c>
-      <c t="s" r="D1" s="1">
+      <c t="s" s="1" r="H1">
         <v>20</v>
       </c>
-      <c t="s" r="E1" s="1">
-        <v>18</v>
-      </c>
-      <c t="s" r="F1" s="1">
-        <v>14</v>
-      </c>
-      <c t="s" r="G1" s="1">
+      <c t="s" s="1" r="I1">
+        <v>22</v>
+      </c>
+    </row>
+    <row spans="1:9" r="2">
+      <c t="s" s="2" r="A2">
+        <v>7</v>
+      </c>
+      <c t="s" s="2" r="B2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="C2">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D2"/>
+      <c t="s" s="2" r="E2">
+        <v>12</v>
+      </c>
+      <c t="b" s="2" r="F2">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G2">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I2"/>
+    </row>
+    <row spans="1:9" r="3">
+      <c t="s" s="2" r="A3">
+        <v>9</v>
+      </c>
+      <c t="s" s="2" r="B3">
+        <v>2</v>
+      </c>
+      <c t="s" s="2" r="C3">
+        <v>13</v>
+      </c>
+      <c t="s" s="2" r="D3">
+        <v>6</v>
+      </c>
+      <c t="s" s="2" r="E3">
+        <v>7</v>
+      </c>
+      <c t="b" s="2" r="F3">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G3">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H3">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I3"/>
+    </row>
+    <row spans="1:9" r="4">
+      <c t="s" s="2" r="A4">
+        <v>10</v>
+      </c>
+      <c t="s" s="2" r="B4">
+        <v>3</v>
+      </c>
+      <c t="s" s="2" r="C4">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D4"/>
+      <c t="s" s="2" r="E4"/>
+      <c t="b" s="2" r="F4">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G4">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H4">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I4"/>
+    </row>
+    <row spans="1:9" r="5">
+      <c t="s" s="2" r="A5">
+        <v>8</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>4</v>
+      </c>
+      <c t="s" s="2" r="C5">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D5"/>
+      <c t="s" s="2" r="E5"/>
+      <c t="b" s="2" r="F5">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G5">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H5">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I5">
         <v>15</v>
       </c>
-      <c t="s" r="H1" s="1">
-        <v>19</v>
-      </c>
     </row>
-    <row spans="1:8" r="2">
-      <c t="s" r="A2" s="2">
+    <row spans="1:9" r="6">
+      <c t="s" s="2" r="A6">
+        <v>11</v>
+      </c>
+      <c t="s" s="2" r="B6">
+        <v>4</v>
+      </c>
+      <c t="s" s="2" r="C6">
+        <v>5</v>
+      </c>
+      <c t="s" s="2" r="D6"/>
+      <c t="s" s="2" r="E6">
         <v>7</v>
       </c>
-      <c t="s" r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c t="s" r="D2" s="2"/>
-      <c t="s" r="E2" s="2">
-        <v>12</v>
-      </c>
-      <c t="b" r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G2" s="2">
+      <c t="b" s="2" r="F6">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G6">
         <v>0</v>
       </c>
-      <c t="b" r="H2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:8" r="3">
-      <c t="s" r="A3" s="2">
-        <v>9</v>
-      </c>
-      <c t="s" r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c t="s" r="C3" s="2">
-        <v>13</v>
-      </c>
-      <c t="s" r="D3" s="2">
-        <v>6</v>
-      </c>
-      <c t="s" r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c t="b" r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c t="b" r="H3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:8" r="4">
-      <c t="s" r="A4" s="2">
-        <v>10</v>
-      </c>
-      <c t="s" r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c t="s" r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c t="s" r="D4" s="2"/>
-      <c t="s" r="E4" s="2"/>
-      <c t="b" r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c t="b" r="H4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:8" r="5">
-      <c t="s" r="A5" s="2">
-        <v>8</v>
-      </c>
-      <c t="s" r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c t="s" r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c t="s" r="D5" s="2"/>
-      <c t="s" r="E5" s="2"/>
-      <c t="b" r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c t="b" r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:8" r="6">
-      <c t="s" r="A6" s="2">
-        <v>11</v>
-      </c>
-      <c t="s" r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c t="s" r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c t="s" r="D6" s="2"/>
-      <c t="s" r="E6" s="2">
-        <v>7</v>
-      </c>
-      <c t="b" r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c t="b" r="H6" s="2">
-        <v>1</v>
-      </c>
+      <c t="b" s="2" r="H6">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
-  <pageMargins bottom="1" top="1" header="0.5" footer="0.5" right="0.75" left="0.75"/>
+  <autoFilter ref="A1:I1"/>
+  <pageMargins bottom="1" right="0.75" footer="0.5" top="1" header="0.5" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added unit tests for manual reordering.
Also fixed typo: MAX_LINE_LENTH => MAX_LINE_LENGTH
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t/>
   </si>
@@ -58,6 +58,10 @@
   <si>
     <t>SYS001
 SYS002:abc123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The foo shall bar all night long!
+</t>
   </si>
   <si>
     <t xml:space="preserve">Unicode: -40° ±1%
@@ -438,184 +442,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft" state="frozen" topLeftCell="A2"/>
-      <selection activeCell="A1" sqref="A1" pane="bottomLeft"/>
+      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5" max="1" min="1"/>
-    <col width="8.5" max="2" min="2"/>
-    <col width="20.5" max="3" min="3"/>
-    <col width="9.5" max="4" min="4"/>
-    <col width="16.5" max="5" min="5"/>
-    <col width="9.5" max="6" min="6"/>
-    <col width="10.5" max="7" min="7"/>
-    <col width="12.5" max="8" min="8"/>
-    <col width="35.5" max="9" min="9"/>
+    <col width="11.5" min="1" max="1"/>
+    <col width="8.5" min="2" max="2"/>
+    <col width="36.5" min="3" max="3"/>
+    <col width="9.5" min="4" max="4"/>
+    <col width="16.5" min="5" max="5"/>
+    <col width="9.5" min="6" max="6"/>
+    <col width="10.5" min="7" max="7"/>
+    <col width="12.5" min="8" max="8"/>
+    <col width="35.5" min="9" max="9"/>
   </cols>
   <sheetData>
     <row spans="1:9" r="1">
-      <c t="s" s="1" r="A1">
+      <c t="s" r="A1" s="1">
+        <v>18</v>
+      </c>
+      <c t="s" r="B1" s="1">
+        <v>19</v>
+      </c>
+      <c t="s" r="C1" s="1">
+        <v>24</v>
+      </c>
+      <c t="s" r="D1" s="1">
+        <v>22</v>
+      </c>
+      <c t="s" r="E1" s="1">
+        <v>20</v>
+      </c>
+      <c t="s" r="F1" s="1">
+        <v>15</v>
+      </c>
+      <c t="s" r="G1" s="1">
         <v>17</v>
       </c>
-      <c t="s" s="1" r="B1">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="C1">
+      <c t="s" r="H1" s="1">
+        <v>21</v>
+      </c>
+      <c t="s" r="I1" s="1">
         <v>23</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>19</v>
-      </c>
-      <c t="s" s="1" r="F1">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="G1">
-        <v>16</v>
-      </c>
-      <c t="s" s="1" r="H1">
-        <v>20</v>
-      </c>
-      <c t="s" s="1" r="I1">
-        <v>22</v>
       </c>
     </row>
     <row spans="1:9" r="2">
-      <c t="s" s="2" r="A2">
+      <c t="s" r="A2" s="2">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="B2">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="C2">
-        <v>5</v>
-      </c>
-      <c t="s" s="2" r="D2"/>
-      <c t="s" s="2" r="E2">
+      <c t="s" r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="C2" s="2">
+        <v>13</v>
+      </c>
+      <c t="s" r="D2" s="2"/>
+      <c t="s" r="E2" s="2">
         <v>12</v>
       </c>
-      <c t="b" s="2" r="F2">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G2">
+      <c t="b" r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G2" s="2">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H2">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I2"/>
+      <c t="b" r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I2" s="2"/>
     </row>
     <row spans="1:9" r="3">
-      <c t="s" s="2" r="A3">
+      <c t="s" r="A3" s="2">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="B3">
+      <c t="s" r="B3" s="2">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="C3">
-        <v>13</v>
-      </c>
-      <c t="s" s="2" r="D3">
+      <c t="s" r="C3" s="2">
+        <v>14</v>
+      </c>
+      <c t="s" r="D3" s="2">
         <v>6</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c t="s" r="E3" s="2">
         <v>7</v>
       </c>
-      <c t="b" s="2" r="F3">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G3">
+      <c t="b" r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G3" s="2">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H3">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I3"/>
+      <c t="b" r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I3" s="2"/>
     </row>
     <row spans="1:9" r="4">
-      <c t="s" s="2" r="A4">
+      <c t="s" r="A4" s="2">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c t="s" r="B4" s="2">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c t="s" r="C4" s="2">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D4"/>
-      <c t="s" s="2" r="E4"/>
-      <c t="b" s="2" r="F4">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G4">
+      <c t="s" r="D4" s="2"/>
+      <c t="s" r="E4" s="2"/>
+      <c t="b" r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G4" s="2">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H4">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I4"/>
+      <c t="b" r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I4" s="2"/>
     </row>
     <row spans="1:9" r="5">
-      <c t="s" s="2" r="A5">
+      <c t="s" r="A5" s="2">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="B5">
+      <c t="s" r="B5" s="2">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c t="s" r="C5" s="2">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D5"/>
-      <c t="s" s="2" r="E5"/>
-      <c t="b" s="2" r="F5">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G5">
+      <c t="s" r="D5" s="2"/>
+      <c t="s" r="E5" s="2"/>
+      <c t="b" r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G5" s="2">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H5">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I5">
-        <v>15</v>
+      <c t="b" r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I5" s="2">
+        <v>16</v>
       </c>
     </row>
     <row spans="1:9" r="6">
-      <c t="s" s="2" r="A6">
+      <c t="s" r="A6" s="2">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="B6">
+      <c t="s" r="B6" s="2">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c t="s" r="C6" s="2">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D6"/>
-      <c t="s" s="2" r="E6">
+      <c t="s" r="D6" s="2"/>
+      <c t="s" r="E6" s="2">
         <v>7</v>
       </c>
-      <c t="b" s="2" r="F6">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G6">
+      <c t="b" r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c t="b" r="G6" s="2">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H6">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I6"/>
+      <c t="b" r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c t="s" r="I6" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins bottom="1" right="0.75" footer="0.5" top="1" header="0.5" left="0.75"/>
+  <pageMargins right="0.75" top="1" left="0.75" bottom="1" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed 'id' and 'identifier' to 'uid' (with case).
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -77,9 +77,6 @@
     <t>derived</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>level</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>uid</t>
   </si>
 </sst>
 </file>
@@ -440,186 +440,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane activePane="bottomLeft" ySplit="1" state="frozen" topLeftCell="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
-    <col width="11.5" min="1" max="1"/>
-    <col width="8.5" min="2" max="2"/>
-    <col width="36.5" min="3" max="3"/>
-    <col width="9.5" min="4" max="4"/>
-    <col width="16.5" min="5" max="5"/>
-    <col width="9.5" min="6" max="6"/>
-    <col width="10.5" min="7" max="7"/>
-    <col width="12.5" min="8" max="8"/>
-    <col width="35.5" min="9" max="9"/>
+    <col min="1" max="1" width="11.5"/>
+    <col min="2" max="2" width="8.5"/>
+    <col min="3" max="3" width="36.5"/>
+    <col min="4" max="4" width="9.5"/>
+    <col min="5" max="5" width="16.5"/>
+    <col min="6" max="6" width="9.5"/>
+    <col min="7" max="7" width="10.5"/>
+    <col min="8" max="8" width="12.5"/>
+    <col min="9" max="9" width="35.5"/>
   </cols>
   <sheetData>
     <row spans="1:9" r="1">
-      <c t="s" r="A1" s="1">
+      <c t="s" s="1" r="A1">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B1">
         <v>18</v>
       </c>
-      <c t="s" r="B1" s="1">
+      <c t="s" s="1" r="C1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="E1">
         <v>19</v>
       </c>
-      <c t="s" r="C1" s="1">
-        <v>24</v>
-      </c>
-      <c t="s" r="D1" s="1">
+      <c t="s" s="1" r="F1">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="I1">
         <v>22</v>
-      </c>
-      <c t="s" r="E1" s="1">
-        <v>20</v>
-      </c>
-      <c t="s" r="F1" s="1">
-        <v>15</v>
-      </c>
-      <c t="s" r="G1" s="1">
-        <v>17</v>
-      </c>
-      <c t="s" r="H1" s="1">
-        <v>21</v>
-      </c>
-      <c t="s" r="I1" s="1">
-        <v>23</v>
       </c>
     </row>
     <row spans="1:9" r="2">
-      <c t="s" r="A2" s="2">
+      <c t="s" s="2" r="A2">
         <v>7</v>
       </c>
-      <c t="s" r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="C2" s="2">
+      <c t="s" s="2" r="B2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="C2">
         <v>13</v>
       </c>
-      <c t="s" r="D2" s="2"/>
-      <c t="s" r="E2" s="2">
+      <c t="s" s="2" r="D2"/>
+      <c t="s" s="2" r="E2">
         <v>12</v>
       </c>
-      <c t="b" r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G2" s="2">
+      <c t="b" s="2" r="F2">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G2">
         <v>0</v>
       </c>
-      <c t="b" r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I2" s="2"/>
+      <c t="b" s="2" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I2"/>
     </row>
     <row spans="1:9" r="3">
-      <c t="s" r="A3" s="2">
+      <c t="s" s="2" r="A3">
         <v>9</v>
       </c>
-      <c t="s" r="B3" s="2">
+      <c t="s" s="2" r="B3">
         <v>2</v>
       </c>
-      <c t="s" r="C3" s="2">
+      <c t="s" s="2" r="C3">
         <v>14</v>
       </c>
-      <c t="s" r="D3" s="2">
+      <c t="s" s="2" r="D3">
         <v>6</v>
       </c>
-      <c t="s" r="E3" s="2">
+      <c t="s" s="2" r="E3">
         <v>7</v>
       </c>
-      <c t="b" r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G3" s="2">
+      <c t="b" s="2" r="F3">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G3">
         <v>0</v>
       </c>
-      <c t="b" r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I3" s="2"/>
+      <c t="b" s="2" r="H3">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I3"/>
     </row>
     <row spans="1:9" r="4">
-      <c t="s" r="A4" s="2">
+      <c t="s" s="2" r="A4">
         <v>10</v>
       </c>
-      <c t="s" r="B4" s="2">
+      <c t="s" s="2" r="B4">
         <v>3</v>
       </c>
-      <c t="s" r="C4" s="2">
+      <c t="s" s="2" r="C4">
         <v>5</v>
       </c>
-      <c t="s" r="D4" s="2"/>
-      <c t="s" r="E4" s="2"/>
-      <c t="b" r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G4" s="2">
+      <c t="s" s="2" r="D4"/>
+      <c t="s" s="2" r="E4"/>
+      <c t="b" s="2" r="F4">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G4">
         <v>0</v>
       </c>
-      <c t="b" r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I4" s="2"/>
+      <c t="b" s="2" r="H4">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I4"/>
     </row>
     <row spans="1:9" r="5">
-      <c t="s" r="A5" s="2">
+      <c t="s" s="2" r="A5">
         <v>8</v>
       </c>
-      <c t="s" r="B5" s="2">
+      <c t="s" s="2" r="B5">
         <v>4</v>
       </c>
-      <c t="s" r="C5" s="2">
+      <c t="s" s="2" r="C5">
         <v>5</v>
       </c>
-      <c t="s" r="D5" s="2"/>
-      <c t="s" r="E5" s="2"/>
-      <c t="b" r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G5" s="2">
+      <c t="s" s="2" r="D5"/>
+      <c t="s" s="2" r="E5"/>
+      <c t="b" s="2" r="F5">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G5">
         <v>0</v>
       </c>
-      <c t="b" r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I5" s="2">
+      <c t="b" s="2" r="H5">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I5">
         <v>16</v>
       </c>
     </row>
     <row spans="1:9" r="6">
-      <c t="s" r="A6" s="2">
+      <c t="s" s="2" r="A6">
         <v>11</v>
       </c>
-      <c t="s" r="B6" s="2">
+      <c t="s" s="2" r="B6">
         <v>4</v>
       </c>
-      <c t="s" r="C6" s="2">
+      <c t="s" s="2" r="C6">
         <v>5</v>
       </c>
-      <c t="s" r="D6" s="2"/>
-      <c t="s" r="E6" s="2">
+      <c t="s" s="2" r="D6"/>
+      <c t="s" s="2" r="E6">
         <v>7</v>
       </c>
-      <c t="b" r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c t="b" r="G6" s="2">
+      <c t="b" s="2" r="F6">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G6">
         <v>0</v>
       </c>
-      <c t="b" r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c t="s" r="I6" s="2"/>
+      <c t="b" s="2" r="H6">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins right="0.75" top="1" left="0.75" bottom="1" footer="0.5" header="0.5"/>
+  <pageMargins left="0.75" footer="0.5" bottom="1" top="1" right="0.75" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Strip text for tabular export
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -34,8 +34,7 @@
     <t>2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello, world!
-</t>
+    <t>Hello, world!</t>
   </si>
   <si>
     <t>REF123</t>
@@ -60,12 +59,10 @@
 SYS002:abc123</t>
   </si>
   <si>
-    <t xml:space="preserve">The foo shall bar all night long!
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unicode: -40° ±1%
-</t>
+    <t>The foo shall bar all night long!</t>
+  </si>
+  <si>
+    <t>Unicode: -40° ±1%</t>
   </si>
   <si>
     <t>active</t>
@@ -442,184 +439,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" ySplit="1" state="frozen" topLeftCell="A2"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5"/>
-    <col min="2" max="2" width="8.5"/>
-    <col min="3" max="3" width="36.5"/>
-    <col min="4" max="4" width="9.5"/>
-    <col min="5" max="5" width="16.5"/>
-    <col min="6" max="6" width="9.5"/>
-    <col min="7" max="7" width="10.5"/>
-    <col min="8" max="8" width="12.5"/>
-    <col min="9" max="9" width="35.5"/>
+    <col width="11.5" max="1" min="1"/>
+    <col width="8.5" max="2" min="2"/>
+    <col width="36.5" max="3" min="3"/>
+    <col width="9.5" max="4" min="4"/>
+    <col width="16.5" max="5" min="5"/>
+    <col width="9.5" max="6" min="6"/>
+    <col width="10.5" max="7" min="7"/>
+    <col width="12.5" max="8" min="8"/>
+    <col width="35.5" max="9" min="9"/>
   </cols>
   <sheetData>
-    <row spans="1:9" r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:9">
+      <c s="1" r="A1" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c s="1" r="B1" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c s="1" r="C1" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c s="1" r="D1" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c s="1" r="E1" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c s="1" r="F1" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c s="1" r="G1" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c s="1" r="H1" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c s="1" r="I1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row spans="1:9" r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:9">
+      <c s="2" r="A2" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="2" r="B2">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="C2">
+      <c s="2" r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c s="2" r="C2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="D2"/>
-      <c t="s" s="2" r="E2">
+      <c s="2" r="D2" t="s"/>
+      <c s="2" r="E2" t="s">
         <v>12</v>
       </c>
-      <c t="b" s="2" r="F2">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G2">
+      <c s="2" r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="G2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H2">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I2"/>
+      <c s="2" r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="I2" t="s"/>
     </row>
-    <row spans="1:9" r="3">
-      <c t="s" s="2" r="A3">
+    <row r="3" spans="1:9">
+      <c s="2" r="A3" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="B3">
+      <c s="2" r="B3" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c s="2" r="C3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c s="2" r="D3" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c s="2" r="E3" t="s">
         <v>7</v>
       </c>
-      <c t="b" s="2" r="F3">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G3">
+      <c s="2" r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="G3" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H3">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I3"/>
+      <c s="2" r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="I3" t="s"/>
     </row>
-    <row spans="1:9" r="4">
-      <c t="s" s="2" r="A4">
+    <row r="4" spans="1:9">
+      <c s="2" r="A4" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c s="2" r="B4" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c s="2" r="C4" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D4"/>
-      <c t="s" s="2" r="E4"/>
-      <c t="b" s="2" r="F4">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G4">
+      <c s="2" r="D4" t="s"/>
+      <c s="2" r="E4" t="s"/>
+      <c s="2" r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="G4" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H4">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I4"/>
+      <c s="2" r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="I4" t="s"/>
     </row>
-    <row spans="1:9" r="5">
-      <c t="s" s="2" r="A5">
+    <row r="5" spans="1:9">
+      <c s="2" r="A5" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="B5">
+      <c s="2" r="B5" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c s="2" r="C5" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D5"/>
-      <c t="s" s="2" r="E5"/>
-      <c t="b" s="2" r="F5">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G5">
+      <c s="2" r="D5" t="s"/>
+      <c s="2" r="E5" t="s"/>
+      <c s="2" r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="G5" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H5">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I5">
+      <c s="2" r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="I5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row spans="1:9" r="6">
-      <c t="s" s="2" r="A6">
+    <row r="6" spans="1:9">
+      <c s="2" r="A6" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="B6">
+      <c s="2" r="B6" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c s="2" r="C6" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="D6"/>
-      <c t="s" s="2" r="E6">
+      <c s="2" r="D6" t="s"/>
+      <c s="2" r="E6" t="s">
         <v>7</v>
       </c>
-      <c t="b" s="2" r="F6">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G6">
+      <c s="2" r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="G6" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H6">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I6"/>
+      <c s="2" r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c s="2" r="I6" t="s"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins left="0.75" footer="0.5" bottom="1" top="1" right="0.75" header="0.5"/>
+  <pageMargins header="0.5" top="1" bottom="1" footer="0.5" left="0.75" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update tests to cover wrapping scenario
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -37,6 +37,9 @@
     <t>Hello, world!</t>
   </si>
   <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
     <t>REF123</t>
   </si>
   <si>
@@ -57,9 +60,6 @@
   <si>
     <t>SYS001
 SYS002:abc123</t>
-  </si>
-  <si>
-    <t>The foo shall bar all night long!</t>
   </si>
   <si>
     <t>Unicode: -40° ±1%</t>
@@ -444,179 +444,179 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" topLeftCell="A2" state="frozen" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection sqref="A1" pane="bottomLeft" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <cols>
-    <col width="11.5" max="1" min="1"/>
-    <col width="8.5" max="2" min="2"/>
-    <col width="36.5" max="3" min="3"/>
-    <col width="9.5" max="4" min="4"/>
-    <col width="16.5" max="5" min="5"/>
-    <col width="9.5" max="6" min="6"/>
-    <col width="10.5" max="7" min="7"/>
-    <col width="12.5" max="8" min="8"/>
-    <col width="35.5" max="9" min="9"/>
+    <col min="1" max="1" width="11.5"/>
+    <col min="2" max="2" width="8.5"/>
+    <col min="3" max="3" width="65"/>
+    <col min="4" max="4" width="9.5"/>
+    <col min="5" max="5" width="16.5"/>
+    <col min="6" max="6" width="9.5"/>
+    <col min="7" max="7" width="10.5"/>
+    <col min="8" max="8" width="12.5"/>
+    <col min="9" max="9" width="35.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c s="1" r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c s="1" r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c s="1" r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c s="1" r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c s="1" r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c s="2" r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c s="2" r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c s="2" r="C2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s"/>
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c s="2" r="D2" t="s"/>
-      <c s="2" r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c s="2" r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="G2" t="b">
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="2" r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="I2" t="s"/>
+      <c r="H2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s"/>
     </row>
     <row r="3" spans="1:9">
-      <c s="2" r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c s="2" r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c s="2" r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c s="2" r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c s="2" r="E3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c s="2" r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="G3" t="b">
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="2" r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="I3" t="s"/>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s"/>
     </row>
     <row r="4" spans="1:9">
-      <c s="2" r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c s="2" r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c s="2" r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c s="2" r="D4" t="s"/>
-      <c s="2" r="E4" t="s"/>
-      <c s="2" r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="G4" t="b">
+      <c r="D4" s="2" t="s"/>
+      <c r="E4" s="2" t="s"/>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="2" r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="I4" t="s"/>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s"/>
     </row>
     <row r="5" spans="1:9">
-      <c s="2" r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c s="2" r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c s="2" r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c s="2" r="D5" t="s"/>
-      <c s="2" r="E5" t="s"/>
-      <c s="2" r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="G5" t="b">
+      <c r="D5" s="2" t="s"/>
+      <c r="E5" s="2" t="s"/>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="2" r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="I5" t="s">
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c s="2" r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c s="2" r="B6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c s="2" r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c s="2" r="D6" t="s"/>
-      <c s="2" r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c s="2" r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="G6" t="b">
+      <c r="D6" s="2" t="s"/>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c s="2" r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c s="2" r="I6" t="s"/>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins header="0.5" top="1" bottom="1" footer="0.5" left="0.75" right="0.75"/>
+  <pageMargins top="1" header="0.5" right="0.75" footer="0.5" bottom="1" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Text is no longer re-wrapped at sentence boundaries
</commit_message>
<xml_diff>
--- a/doorstop/core/test/files/exported.xlsx
+++ b/doorstop/core/test/files/exported.xlsx
@@ -17,82 +17,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
-  <si>
-    <t/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>derived</t>
+  </si>
+  <si>
+    <t>normative</t>
+  </si>
+  <si>
+    <t>reviewed</t>
+  </si>
+  <si>
+    <t>REQ001</t>
   </si>
   <si>
     <t>1.2.3</t>
   </si>
   <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Hello, world!</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>REF123</t>
-  </si>
-  <si>
-    <t>REQ001</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>REQ003</t>
-  </si>
-  <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>REQ2-001</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
+tempor incididunt ut labore et dolore magna aliqua.
+Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
+aliquip ex ea commodo consequat.
+Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
+eu fugiat nulla pariatur.
+Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
+deserunt mollit anim id est laborum.</t>
   </si>
   <si>
     <t>SYS001
 SYS002:abc123</t>
   </si>
   <si>
+    <t>REQ003</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
     <t>Unicode: -40° ±1%</t>
   </si>
   <si>
-    <t>active</t>
+    <t>REF123</t>
+  </si>
+  <si>
+    <t>REQ004</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Hello, world!</t>
+  </si>
+  <si>
+    <t>REQ002</t>
+  </si>
+  <si>
+    <t>2.1</t>
   </si>
   <si>
     <t>b5fbcc355112791bbcd2ea881c7c5f81</t>
   </si>
   <si>
-    <t>derived</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>normative</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>reviewed</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>uid</t>
+    <t>REQ2-001</t>
   </si>
 </sst>
 </file>
@@ -136,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -437,7 +441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -445,178 +449,178 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection sqref="A1" pane="bottomLeft" activeCell="A1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5"/>
-    <col min="2" max="2" width="8.5"/>
-    <col min="3" max="3" width="65"/>
-    <col min="4" max="4" width="9.5"/>
-    <col min="5" max="5" width="16.5"/>
-    <col min="6" max="6" width="9.5"/>
-    <col min="7" max="7" width="10.5"/>
-    <col min="8" max="8" width="12.5"/>
-    <col min="9" max="9" width="35.5"/>
+    <col customWidth="1" max="1" min="1" width="11.5"/>
+    <col customWidth="1" max="2" min="2" width="8.5"/>
+    <col customWidth="1" max="3" min="3" width="65"/>
+    <col customWidth="1" max="4" min="4" width="9.5"/>
+    <col customWidth="1" max="5" min="5" width="16.5"/>
+    <col customWidth="1" max="6" min="6" width="9.5"/>
+    <col customWidth="1" max="7" min="7" width="10.5"/>
+    <col customWidth="1" max="8" min="8" width="12.5"/>
+    <col customWidth="1" max="9" min="9" width="35.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row spans="1:9" r="1">
+      <c t="s" s="1" r="A1">
+        <v>0</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row spans="1:9" r="2">
+      <c t="s" s="2" r="A2">
+        <v>9</v>
+      </c>
+      <c t="s" s="2" r="B2">
+        <v>10</v>
+      </c>
+      <c t="s" s="2" r="C2">
+        <v>11</v>
+      </c>
+      <c t="s" s="2" r="D2"/>
+      <c t="s" s="2" r="E2">
+        <v>12</v>
+      </c>
+      <c t="b" s="2" r="F2">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G2">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H2">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I2"/>
+    </row>
+    <row spans="1:9" r="3">
+      <c t="s" s="2" r="A3">
+        <v>13</v>
+      </c>
+      <c t="s" s="2" r="B3">
+        <v>14</v>
+      </c>
+      <c t="s" s="2" r="C3">
+        <v>15</v>
+      </c>
+      <c t="s" s="2" r="D3">
+        <v>16</v>
+      </c>
+      <c t="s" s="2" r="E3">
+        <v>9</v>
+      </c>
+      <c t="b" s="2" r="F3">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G3">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H3">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I3"/>
+    </row>
+    <row spans="1:9" r="4">
+      <c t="s" s="2" r="A4">
+        <v>17</v>
+      </c>
+      <c t="s" s="2" r="B4">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c t="s" s="2" r="C4">
+        <v>19</v>
+      </c>
+      <c t="s" s="2" r="D4"/>
+      <c t="s" s="2" r="E4"/>
+      <c t="b" s="2" r="F4">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G4">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H4">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I4"/>
+    </row>
+    <row spans="1:9" r="5">
+      <c t="s" s="2" r="A5">
+        <v>20</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>21</v>
+      </c>
+      <c t="s" s="2" r="C5">
+        <v>19</v>
+      </c>
+      <c t="s" s="2" r="D5"/>
+      <c t="s" s="2" r="E5"/>
+      <c t="b" s="2" r="F5">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G5">
+        <v>0</v>
+      </c>
+      <c t="b" s="2" r="H5">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I5">
+        <v>22</v>
+      </c>
+    </row>
+    <row spans="1:9" r="6">
+      <c t="s" s="2" r="A6">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c t="s" s="2" r="B6">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c t="s" s="2" r="C6">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
+      <c t="s" s="2" r="D6"/>
+      <c t="s" s="2" r="E6">
+        <v>9</v>
+      </c>
+      <c t="b" s="2" r="F6">
+        <v>1</v>
+      </c>
+      <c t="b" s="2" r="G6">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s"/>
+      <c t="b" s="2" r="H6">
+        <v>1</v>
+      </c>
+      <c t="s" s="2" r="I6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins top="1" header="0.5" right="0.75" footer="0.5" bottom="1" left="0.75"/>
+  <pageMargins footer="0.5" top="1" bottom="1" left="0.75" header="0.5" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>